<commit_message>
update algorithms to include V2
</commit_message>
<xml_diff>
--- a/analysis/ec2/1_outputs/rf_predict.xlsx
+++ b/analysis/ec2/1_outputs/rf_predict.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunwookang/Desktop/research/ecig/analysis/ec2/1_outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D47A69-514D-9449-B381-1D846A1F42FC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8356C3D-D384-3B4B-9BC7-DDA3BCE7D512}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="25440" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5360" yWindow="460" windowWidth="20240" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rf_predict" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>Index</t>
   </si>
@@ -191,6 +192,9 @@
   </si>
   <si>
     <t>m/z: 2914 importance: 0.0141</t>
+  </si>
+  <si>
+    <t>old</t>
   </si>
 </sst>
 </file>
@@ -921,6 +925,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-D146-1B4F-996B-5264A6B4EEBA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -936,6 +945,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-D146-1B4F-996B-5264A6B4EEBA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -951,6 +965,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-D146-1B4F-996B-5264A6B4EEBA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -966,6 +985,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-D146-1B4F-996B-5264A6B4EEBA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -981,6 +1005,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-D146-1B4F-996B-5264A6B4EEBA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -1018,6 +1047,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-D146-1B4F-996B-5264A6B4EEBA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -1035,6 +1069,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-D146-1B4F-996B-5264A6B4EEBA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -1044,6 +1083,16 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-543A-AE4C-B05F-95E1A21E187A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-D146-1B4F-996B-5264A6B4EEBA}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1142,28 +1191,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2168,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:C44"/>
+    <sheetView tabSelected="1" topLeftCell="F26" workbookViewId="0">
+      <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2696,7 +2745,7 @@
         <v>7</v>
       </c>
       <c r="I30" s="2">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -2713,7 +2762,7 @@
         <v>9</v>
       </c>
       <c r="I31" s="3">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -2730,7 +2779,7 @@
         <v>11</v>
       </c>
       <c r="I32" s="4">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -2764,7 +2813,7 @@
         <v>15</v>
       </c>
       <c r="I34" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -2798,7 +2847,7 @@
         <v>19</v>
       </c>
       <c r="I36" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2815,7 +2864,7 @@
         <v>21</v>
       </c>
       <c r="I37" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2827,7 +2876,7 @@
       <c r="D38" s="3"/>
       <c r="I38">
         <f>SUM(I30:I37)</f>
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2869,6 +2918,9 @@
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
+      <c r="G43" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="11" t="s">
@@ -2877,6 +2929,15 @@
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
+      <c r="G44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I44" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="11" t="s">
@@ -2885,6 +2946,15 @@
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
+      <c r="G45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I45" s="3">
+        <v>7</v>
+      </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="11" t="s">
@@ -2893,6 +2963,15 @@
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
+      <c r="G46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" s="4">
+        <v>12</v>
+      </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="11" t="s">
@@ -2901,6 +2980,15 @@
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
+      <c r="G47" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="11" t="s">
@@ -2909,40 +2997,80 @@
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="G48" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="G49" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H49" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I49" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="G50" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I50" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="G51" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I51" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="I52">
+        <f>SUM(I44:I51)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" s="11" t="s">
         <v>46</v>
       </c>
@@ -2950,7 +3078,7 @@
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:9">
       <c r="A54" s="12" t="s">
         <v>47</v>
       </c>
@@ -2958,7 +3086,7 @@
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:9">
       <c r="A55" s="12" t="s">
         <v>48</v>
       </c>
@@ -2966,7 +3094,7 @@
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:9">
       <c r="A56" s="12" t="s">
         <v>49</v>
       </c>
@@ -2974,7 +3102,7 @@
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:9">
       <c r="A57" s="13" t="s">
         <v>50</v>
       </c>
@@ -2982,7 +3110,7 @@
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:9">
       <c r="A58" s="13" t="s">
         <v>51</v>
       </c>
@@ -2990,7 +3118,7 @@
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:9">
       <c r="A59" s="16" t="s">
         <v>52</v>
       </c>
@@ -2998,7 +3126,7 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:9">
       <c r="A60" s="16" t="s">
         <v>53</v>
       </c>
@@ -3006,7 +3134,7 @@
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:9">
       <c r="A61" s="16" t="s">
         <v>54</v>
       </c>
@@ -3014,7 +3142,7 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:9">
       <c r="A62" s="16" t="s">
         <v>55</v>
       </c>
@@ -3022,7 +3150,7 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:9">
       <c r="A63" s="17" t="s">
         <v>56</v>
       </c>
@@ -3034,4 +3162,16 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B43A19-62D1-B840-A2EF-566900EA6D4E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>